<commit_message>
Fix xlsx converter script and broken xlsx files
</commit_message>
<xml_diff>
--- a/app/config/tables/femaleClients/forms/screenClient/screenClient.xlsx
+++ b/app/config/tables/femaleClients/forms/screenClient/screenClient.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26330"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\toolsuite\app-designer\app\config\tables\femaleClients\forms\screenClient\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="236" yWindow="236" windowWidth="25357" windowHeight="15814" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15820" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -799,9 +794,6 @@
     <t>condition</t>
   </si>
   <si>
-    <t>else</t>
-  </si>
-  <si>
     <t>end if // screening</t>
   </si>
   <si>
@@ -853,16 +845,19 @@
     <t>if // ref_reason</t>
   </si>
   <si>
-    <t>selected(data('refusal_reasons','a9')</t>
-  </si>
-  <si>
     <t>end if // ref_reason</t>
+  </si>
+  <si>
+    <t>selected(data('refusal_reasons','a9'))</t>
+  </si>
+  <si>
+    <t>else // screening</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -2473,35 +2468,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S114"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="G38" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="6" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B49" sqref="B49"/>
+      <selection pane="bottomRight" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="15.44140625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="21.44140625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="41.21875" style="3" customWidth="1"/>
+    <col min="1" max="1" width="15.5" style="3" customWidth="1"/>
+    <col min="2" max="2" width="21.5" style="3" customWidth="1"/>
+    <col min="3" max="3" width="41.1640625" style="3" customWidth="1"/>
     <col min="4" max="4" width="13.6640625" style="8" customWidth="1"/>
-    <col min="5" max="5" width="24.44140625" style="18" customWidth="1"/>
-    <col min="6" max="6" width="25.109375" style="21" customWidth="1"/>
+    <col min="5" max="5" width="24.5" style="18" customWidth="1"/>
+    <col min="6" max="6" width="25.1640625" style="21" customWidth="1"/>
     <col min="7" max="7" width="63" style="3" customWidth="1"/>
-    <col min="8" max="8" width="22.77734375" style="3" customWidth="1"/>
-    <col min="9" max="10" width="10.77734375" style="3"/>
-    <col min="11" max="11" width="10.77734375" style="23"/>
-    <col min="12" max="12" width="10.77734375" style="3"/>
+    <col min="8" max="8" width="22.83203125" style="3" customWidth="1"/>
+    <col min="9" max="10" width="10.83203125" style="3"/>
+    <col min="11" max="11" width="10.83203125" style="23"/>
+    <col min="12" max="12" width="10.83203125" style="3"/>
     <col min="13" max="13" width="15" style="3" customWidth="1"/>
-    <col min="14" max="14" width="10.77734375" style="3"/>
+    <col min="14" max="14" width="10.83203125" style="3"/>
     <col min="15" max="15" width="28" style="3" customWidth="1"/>
-    <col min="16" max="16384" width="10.77734375" style="3"/>
+    <col min="16" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="5" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" s="5" customFormat="1" ht="30">
       <c r="A1" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>199</v>
@@ -2558,7 +2553,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" s="11" customFormat="1">
       <c r="D2" s="10" t="s">
         <v>12</v>
       </c>
@@ -2573,7 +2568,7 @@
       <c r="J2" s="12"/>
       <c r="K2" s="30"/>
     </row>
-    <row r="3" spans="1:19" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" s="13" customFormat="1">
       <c r="D3" s="8" t="s">
         <v>13</v>
       </c>
@@ -2586,7 +2581,7 @@
       </c>
       <c r="K3" s="31"/>
     </row>
-    <row r="4" spans="1:19" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" s="13" customFormat="1">
       <c r="D4" s="8" t="s">
         <v>14</v>
       </c>
@@ -2599,7 +2594,7 @@
       </c>
       <c r="K4" s="31"/>
     </row>
-    <row r="5" spans="1:19" s="13" customFormat="1" ht="125.7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" s="13" customFormat="1" ht="120">
       <c r="D5" s="10" t="s">
         <v>16</v>
       </c>
@@ -2612,7 +2607,7 @@
       </c>
       <c r="K5" s="31"/>
     </row>
-    <row r="6" spans="1:19" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" s="13" customFormat="1">
       <c r="D6" s="8" t="s">
         <v>185</v>
       </c>
@@ -2629,19 +2624,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:19" s="13" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" s="13" customFormat="1">
       <c r="B7" s="13" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D7" s="8"/>
       <c r="E7" s="18"/>
       <c r="F7" s="21"/>
       <c r="K7" s="31"/>
     </row>
-    <row r="8" spans="1:19" s="13" customFormat="1" ht="47.15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" s="13" customFormat="1" ht="45">
       <c r="D8" s="8" t="s">
         <v>16</v>
       </c>
@@ -2657,16 +2652,16 @@
       </c>
       <c r="K8" s="31"/>
     </row>
-    <row r="9" spans="1:19" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" s="13" customFormat="1">
       <c r="B9" s="13" t="s">
-        <v>256</v>
+        <v>275</v>
       </c>
       <c r="D9" s="8"/>
       <c r="E9" s="18"/>
       <c r="F9" s="21"/>
       <c r="K9" s="31"/>
     </row>
-    <row r="10" spans="1:19" s="13" customFormat="1" ht="78.55" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" s="13" customFormat="1" ht="75">
       <c r="D10" s="8" t="s">
         <v>13</v>
       </c>
@@ -2684,19 +2679,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:19" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" s="13" customFormat="1">
       <c r="B11" s="13" t="s">
+        <v>261</v>
+      </c>
+      <c r="C11" s="13" t="s">
         <v>262</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>263</v>
       </c>
       <c r="D11" s="8"/>
       <c r="E11" s="18"/>
       <c r="F11" s="21"/>
       <c r="K11" s="31"/>
     </row>
-    <row r="12" spans="1:19" s="13" customFormat="1" ht="47.15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" s="13" customFormat="1" ht="45">
       <c r="D12" s="8" t="s">
         <v>185</v>
       </c>
@@ -2716,19 +2711,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:19" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" s="13" customFormat="1">
       <c r="B13" s="13" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D13" s="8"/>
       <c r="E13" s="18"/>
       <c r="F13" s="21"/>
       <c r="K13" s="31"/>
     </row>
-    <row r="14" spans="1:19" s="13" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" s="13" customFormat="1" ht="30">
       <c r="D14" s="8" t="s">
         <v>13</v>
       </c>
@@ -2742,7 +2737,7 @@
       <c r="K14" s="31"/>
       <c r="N14" s="14"/>
     </row>
-    <row r="15" spans="1:19" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" s="13" customFormat="1">
       <c r="B15" s="13" t="s">
         <v>200</v>
       </c>
@@ -2752,7 +2747,7 @@
       <c r="K15" s="31"/>
       <c r="N15" s="14"/>
     </row>
-    <row r="16" spans="1:19" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" s="13" customFormat="1">
       <c r="D16" s="8" t="s">
         <v>185</v>
       </c>
@@ -2767,7 +2762,7 @@
       </c>
       <c r="K16" s="31"/>
     </row>
-    <row r="17" spans="2:11" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:11" s="13" customFormat="1">
       <c r="D17" s="8" t="s">
         <v>12</v>
       </c>
@@ -2780,7 +2775,7 @@
       </c>
       <c r="K17" s="31"/>
     </row>
-    <row r="18" spans="2:11" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:11" s="13" customFormat="1">
       <c r="D18" s="8" t="s">
         <v>186</v>
       </c>
@@ -2795,7 +2790,7 @@
       </c>
       <c r="K18" s="32"/>
     </row>
-    <row r="19" spans="2:11" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:11" s="13" customFormat="1">
       <c r="D19" s="8" t="s">
         <v>185</v>
       </c>
@@ -2810,7 +2805,7 @@
       </c>
       <c r="K19" s="32"/>
     </row>
-    <row r="20" spans="2:11" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:11" s="13" customFormat="1">
       <c r="D20" s="8" t="s">
         <v>12</v>
       </c>
@@ -2823,7 +2818,7 @@
       </c>
       <c r="K20" s="31"/>
     </row>
-    <row r="21" spans="2:11" s="13" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:11" s="13" customFormat="1" ht="30">
       <c r="D21" s="8" t="s">
         <v>187</v>
       </c>
@@ -2838,7 +2833,7 @@
       </c>
       <c r="K21" s="31"/>
     </row>
-    <row r="22" spans="2:11" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:11" s="13" customFormat="1">
       <c r="D22" s="8" t="s">
         <v>12</v>
       </c>
@@ -2851,7 +2846,7 @@
       </c>
       <c r="K22" s="31"/>
     </row>
-    <row r="23" spans="2:11" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:11" s="13" customFormat="1">
       <c r="B23" s="13" t="s">
         <v>201</v>
       </c>
@@ -2860,7 +2855,7 @@
       <c r="F23" s="21"/>
       <c r="K23" s="31"/>
     </row>
-    <row r="24" spans="2:11" s="13" customFormat="1" ht="62.85" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:11" s="13" customFormat="1" ht="60">
       <c r="D24" s="8" t="s">
         <v>185</v>
       </c>
@@ -2880,19 +2875,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="2:11" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:11" s="13" customFormat="1">
       <c r="B25" s="13" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C25" s="13" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D25" s="8"/>
       <c r="E25" s="18"/>
       <c r="F25" s="21"/>
       <c r="K25" s="32"/>
     </row>
-    <row r="26" spans="2:11" s="13" customFormat="1" ht="94.25" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:11" s="13" customFormat="1" ht="90">
       <c r="D26" s="8" t="s">
         <v>13</v>
       </c>
@@ -2911,12 +2906,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="2:11" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:11" s="13" customFormat="1">
       <c r="B27" s="13" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C27" s="13" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D27" s="8"/>
       <c r="E27" s="18"/>
@@ -2924,7 +2919,7 @@
       <c r="J27" s="16"/>
       <c r="K27" s="31"/>
     </row>
-    <row r="28" spans="2:11" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:11" s="13" customFormat="1">
       <c r="D28" s="8" t="s">
         <v>13</v>
       </c>
@@ -2937,7 +2932,7 @@
       </c>
       <c r="K28" s="32"/>
     </row>
-    <row r="29" spans="2:11" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:11" s="13" customFormat="1">
       <c r="D29" s="8" t="s">
         <v>13</v>
       </c>
@@ -2950,7 +2945,7 @@
       </c>
       <c r="K29" s="32"/>
     </row>
-    <row r="30" spans="2:11" s="13" customFormat="1" ht="62.85" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:11" s="13" customFormat="1" ht="60">
       <c r="D30" s="8" t="s">
         <v>185</v>
       </c>
@@ -2970,19 +2965,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="2:11" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:11" s="13" customFormat="1">
       <c r="B31" s="13" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C31" s="13" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D31" s="8"/>
       <c r="E31" s="18"/>
       <c r="F31" s="21"/>
       <c r="K31" s="32"/>
     </row>
-    <row r="32" spans="2:11" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:11" s="13" customFormat="1">
       <c r="D32" s="8" t="s">
         <v>185</v>
       </c>
@@ -2997,7 +2992,7 @@
       </c>
       <c r="K32" s="32"/>
     </row>
-    <row r="33" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" s="13" customFormat="1">
       <c r="D33" s="8" t="s">
         <v>185</v>
       </c>
@@ -3012,7 +3007,7 @@
       </c>
       <c r="K33" s="32"/>
     </row>
-    <row r="34" spans="1:11" s="13" customFormat="1" ht="47.15" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" s="13" customFormat="1" ht="45">
       <c r="D34" s="9" t="s">
         <v>16</v>
       </c>
@@ -3028,7 +3023,7 @@
       </c>
       <c r="K34" s="31"/>
     </row>
-    <row r="35" spans="1:11" s="13" customFormat="1" ht="47.15" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" s="13" customFormat="1" ht="60">
       <c r="D35" s="9" t="s">
         <v>185</v>
       </c>
@@ -3046,19 +3041,19 @@
       </c>
       <c r="K35" s="31"/>
     </row>
-    <row r="36" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" s="13" customFormat="1">
       <c r="B36" s="13" t="s">
+        <v>268</v>
+      </c>
+      <c r="C36" s="13" t="s">
         <v>269</v>
-      </c>
-      <c r="C36" s="13" t="s">
-        <v>270</v>
       </c>
       <c r="D36" s="9"/>
       <c r="E36" s="19"/>
       <c r="F36" s="21"/>
       <c r="K36" s="31"/>
     </row>
-    <row r="37" spans="1:11" s="13" customFormat="1" ht="47.15" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" s="13" customFormat="1" ht="45">
       <c r="D37" s="8" t="s">
         <v>13</v>
       </c>
@@ -3076,7 +3071,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" s="13" customFormat="1">
       <c r="D38" s="8" t="s">
         <v>185</v>
       </c>
@@ -3093,27 +3088,27 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" s="13" customFormat="1">
       <c r="B39" s="3" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D39" s="8"/>
       <c r="E39" s="18"/>
       <c r="F39" s="21"/>
       <c r="K39" s="31"/>
     </row>
-    <row r="40" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" s="13" customFormat="1">
       <c r="B40" s="13" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D40" s="8"/>
       <c r="E40" s="18"/>
       <c r="F40" s="21"/>
       <c r="K40" s="32"/>
     </row>
-    <row r="41" spans="1:11" s="13" customFormat="1" ht="62.85" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" s="13" customFormat="1" ht="60">
       <c r="A41" s="13" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D41" s="9" t="s">
         <v>16</v>
@@ -3127,18 +3122,18 @@
       </c>
       <c r="K41" s="31"/>
     </row>
-    <row r="42" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" s="13" customFormat="1">
       <c r="B42" s="13" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D42" s="9"/>
       <c r="E42" s="19"/>
       <c r="F42" s="21"/>
       <c r="K42" s="31"/>
     </row>
-    <row r="43" spans="1:11" s="13" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" s="13" customFormat="1" ht="30">
       <c r="A43" s="13" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D43" s="8" t="s">
         <v>188</v>
@@ -3154,9 +3149,9 @@
       </c>
       <c r="K43" s="32"/>
     </row>
-    <row r="44" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" s="13" customFormat="1">
       <c r="B44" s="13" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C44" s="13" t="s">
         <v>274</v>
@@ -3166,7 +3161,7 @@
       <c r="F44" s="21"/>
       <c r="K44" s="32"/>
     </row>
-    <row r="45" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" s="13" customFormat="1">
       <c r="D45" s="8" t="s">
         <v>12</v>
       </c>
@@ -3179,16 +3174,16 @@
       </c>
       <c r="K45" s="32"/>
     </row>
-    <row r="46" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" s="13" customFormat="1">
       <c r="B46" s="13" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D46" s="8"/>
       <c r="E46" s="18"/>
       <c r="F46" s="21"/>
       <c r="K46" s="32"/>
     </row>
-    <row r="47" spans="1:11" s="13" customFormat="1" ht="62.85" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" s="13" customFormat="1" ht="60">
       <c r="D47" s="9" t="s">
         <v>16</v>
       </c>
@@ -3201,18 +3196,18 @@
       </c>
       <c r="K47" s="31"/>
     </row>
-    <row r="48" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" s="13" customFormat="1">
       <c r="B48" s="13" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D48" s="8"/>
       <c r="E48" s="18"/>
       <c r="F48" s="21"/>
       <c r="K48" s="31"/>
     </row>
-    <row r="49" spans="1:11" s="13" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" s="13" customFormat="1" ht="30">
       <c r="A49" s="13" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D49" s="8" t="s">
         <v>16</v>
@@ -3226,199 +3221,199 @@
       </c>
       <c r="K49" s="31"/>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11">
       <c r="K50" s="33"/>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11">
       <c r="K51" s="33"/>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11">
       <c r="K52" s="33"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11">
       <c r="K53" s="33"/>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11">
       <c r="K54" s="33"/>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11">
       <c r="K55" s="33"/>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11">
       <c r="K56" s="33"/>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11">
       <c r="K57" s="33"/>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11">
       <c r="K58" s="33"/>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11">
       <c r="K59" s="33"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11">
       <c r="K60" s="33"/>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:11">
       <c r="K61" s="33"/>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:11">
       <c r="K62" s="33"/>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:11">
       <c r="K63" s="33"/>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:11">
       <c r="K64" s="33"/>
     </row>
-    <row r="65" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="65" spans="11:11">
       <c r="K65" s="33"/>
     </row>
-    <row r="66" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="66" spans="11:11">
       <c r="K66" s="33"/>
     </row>
-    <row r="67" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="67" spans="11:11">
       <c r="K67" s="33"/>
     </row>
-    <row r="68" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="68" spans="11:11">
       <c r="K68" s="33"/>
     </row>
-    <row r="69" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="69" spans="11:11">
       <c r="K69" s="33"/>
     </row>
-    <row r="70" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="70" spans="11:11">
       <c r="K70" s="33"/>
     </row>
-    <row r="71" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="71" spans="11:11">
       <c r="K71" s="33"/>
     </row>
-    <row r="72" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="72" spans="11:11">
       <c r="K72" s="33"/>
     </row>
-    <row r="73" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="73" spans="11:11">
       <c r="K73" s="33"/>
     </row>
-    <row r="74" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="74" spans="11:11">
       <c r="K74" s="33"/>
     </row>
-    <row r="75" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="75" spans="11:11">
       <c r="K75" s="33"/>
     </row>
-    <row r="76" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="76" spans="11:11">
       <c r="K76" s="33"/>
     </row>
-    <row r="77" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="77" spans="11:11">
       <c r="K77" s="33"/>
     </row>
-    <row r="78" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="78" spans="11:11">
       <c r="K78" s="33"/>
     </row>
-    <row r="79" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="79" spans="11:11">
       <c r="K79" s="33"/>
     </row>
-    <row r="80" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="80" spans="11:11">
       <c r="K80" s="33"/>
     </row>
-    <row r="81" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="81" spans="11:11">
       <c r="K81" s="33"/>
     </row>
-    <row r="82" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="82" spans="11:11">
       <c r="K82" s="33"/>
     </row>
-    <row r="83" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="83" spans="11:11">
       <c r="K83" s="33"/>
     </row>
-    <row r="84" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="84" spans="11:11">
       <c r="K84" s="33"/>
     </row>
-    <row r="85" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="85" spans="11:11">
       <c r="K85" s="33"/>
     </row>
-    <row r="86" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="86" spans="11:11">
       <c r="K86" s="33"/>
     </row>
-    <row r="87" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="87" spans="11:11">
       <c r="K87" s="33"/>
     </row>
-    <row r="88" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="88" spans="11:11">
       <c r="K88" s="33"/>
     </row>
-    <row r="89" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="89" spans="11:11">
       <c r="K89" s="33"/>
     </row>
-    <row r="90" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="90" spans="11:11">
       <c r="K90" s="33"/>
     </row>
-    <row r="91" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="91" spans="11:11">
       <c r="K91" s="33"/>
     </row>
-    <row r="92" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="92" spans="11:11">
       <c r="K92" s="33"/>
     </row>
-    <row r="93" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="93" spans="11:11">
       <c r="K93" s="33"/>
     </row>
-    <row r="94" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="94" spans="11:11">
       <c r="K94" s="33"/>
     </row>
-    <row r="95" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="95" spans="11:11">
       <c r="K95" s="33"/>
     </row>
-    <row r="96" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="96" spans="11:11">
       <c r="K96" s="33"/>
     </row>
-    <row r="97" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="97" spans="11:11">
       <c r="K97" s="33"/>
     </row>
-    <row r="98" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="98" spans="11:11">
       <c r="K98" s="33"/>
     </row>
-    <row r="99" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="99" spans="11:11">
       <c r="K99" s="33"/>
     </row>
-    <row r="100" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="100" spans="11:11">
       <c r="K100" s="33"/>
     </row>
-    <row r="101" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="101" spans="11:11">
       <c r="K101" s="33"/>
     </row>
-    <row r="102" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="102" spans="11:11">
       <c r="K102" s="33"/>
     </row>
-    <row r="103" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="103" spans="11:11">
       <c r="K103" s="33"/>
     </row>
-    <row r="104" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="104" spans="11:11">
       <c r="K104" s="33"/>
     </row>
-    <row r="105" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="105" spans="11:11">
       <c r="K105" s="33"/>
     </row>
-    <row r="106" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="106" spans="11:11">
       <c r="K106" s="33"/>
     </row>
-    <row r="107" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="107" spans="11:11">
       <c r="K107" s="33"/>
     </row>
-    <row r="108" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="108" spans="11:11">
       <c r="K108" s="33"/>
     </row>
-    <row r="109" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="109" spans="11:11">
       <c r="K109" s="33"/>
     </row>
-    <row r="110" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="110" spans="11:11">
       <c r="K110" s="33"/>
     </row>
-    <row r="111" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="111" spans="11:11">
       <c r="K111" s="33"/>
     </row>
-    <row r="112" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="112" spans="11:11">
       <c r="K112" s="33"/>
     </row>
-    <row r="113" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="113" spans="11:11">
       <c r="K113" s="33"/>
     </row>
-    <row r="114" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="114" spans="11:11">
       <c r="K114" s="33"/>
     </row>
   </sheetData>
@@ -3440,15 +3435,15 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="21.44140625" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="21.5" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="25.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="21.44140625" style="2"/>
-    <col min="3" max="3" width="42.109375" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="21.44140625" style="2"/>
+    <col min="2" max="2" width="21.5" style="2"/>
+    <col min="3" max="3" width="42.1640625" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="21.5" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>189</v>
       </c>
@@ -3459,7 +3454,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
         <v>17</v>
       </c>
@@ -3470,7 +3465,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
         <v>17</v>
       </c>
@@ -3481,7 +3476,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
         <v>121</v>
       </c>
@@ -3492,7 +3487,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
         <v>121</v>
       </c>
@@ -3503,7 +3498,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
         <v>121</v>
       </c>
@@ -3514,7 +3509,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3">
       <c r="A7" s="2" t="s">
         <v>122</v>
       </c>
@@ -3525,7 +3520,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3">
       <c r="A8" s="2" t="s">
         <v>22</v>
       </c>
@@ -3536,7 +3531,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3">
       <c r="A9" s="2" t="s">
         <v>22</v>
       </c>
@@ -3547,7 +3542,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3">
       <c r="A10" s="2" t="s">
         <v>22</v>
       </c>
@@ -3558,7 +3553,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3">
       <c r="A11" s="2" t="s">
         <v>22</v>
       </c>
@@ -3569,7 +3564,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3">
       <c r="A12" s="2" t="s">
         <v>22</v>
       </c>
@@ -3580,7 +3575,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3">
       <c r="A13" s="2" t="s">
         <v>22</v>
       </c>
@@ -3591,7 +3586,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3">
       <c r="A14" s="2" t="s">
         <v>22</v>
       </c>
@@ -3602,7 +3597,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3">
       <c r="A15" s="2" t="s">
         <v>22</v>
       </c>
@@ -3613,7 +3608,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3">
       <c r="A16" s="2" t="s">
         <v>29</v>
       </c>
@@ -3624,7 +3619,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3">
       <c r="A17" s="2" t="s">
         <v>29</v>
       </c>
@@ -3635,7 +3630,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3">
       <c r="A18" s="2" t="s">
         <v>29</v>
       </c>
@@ -3646,7 +3641,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3">
       <c r="A19" s="2" t="s">
         <v>29</v>
       </c>
@@ -3657,7 +3652,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3">
       <c r="A20" s="2" t="s">
         <v>29</v>
       </c>
@@ -3668,7 +3663,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3">
       <c r="A21" s="2" t="s">
         <v>29</v>
       </c>
@@ -3679,7 +3674,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3">
       <c r="A22" s="2" t="s">
         <v>29</v>
       </c>
@@ -3690,7 +3685,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3">
       <c r="A23" s="2" t="s">
         <v>29</v>
       </c>
@@ -3701,7 +3696,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3">
       <c r="A24" s="2" t="s">
         <v>29</v>
       </c>
@@ -3712,7 +3707,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3">
       <c r="A25" s="2" t="s">
         <v>29</v>
       </c>
@@ -3723,7 +3718,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3">
       <c r="A26" s="2" t="s">
         <v>29</v>
       </c>
@@ -3734,7 +3729,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3">
       <c r="A27" s="2" t="s">
         <v>130</v>
       </c>
@@ -3745,7 +3740,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3">
       <c r="A28" s="2" t="s">
         <v>130</v>
       </c>
@@ -3756,7 +3751,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3">
       <c r="A29" s="2" t="s">
         <v>130</v>
       </c>
@@ -3767,7 +3762,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3">
       <c r="A30" s="2" t="s">
         <v>130</v>
       </c>
@@ -3778,7 +3773,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3">
       <c r="A31" s="2" t="s">
         <v>130</v>
       </c>
@@ -3789,7 +3784,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3">
       <c r="A32" s="2" t="s">
         <v>130</v>
       </c>
@@ -3800,7 +3795,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3">
       <c r="A33" s="2" t="s">
         <v>130</v>
       </c>
@@ -3811,7 +3806,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3">
       <c r="A34" s="2" t="s">
         <v>130</v>
       </c>
@@ -3822,7 +3817,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3">
       <c r="A35" s="2" t="s">
         <v>130</v>
       </c>
@@ -3833,7 +3828,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3">
       <c r="A36" s="2" t="s">
         <v>130</v>
       </c>
@@ -3844,7 +3839,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3">
       <c r="A37" s="2" t="s">
         <v>130</v>
       </c>
@@ -3855,7 +3850,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3">
       <c r="A38" s="2" t="s">
         <v>48</v>
       </c>
@@ -3866,7 +3861,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3">
       <c r="A39" s="2" t="s">
         <v>48</v>
       </c>
@@ -3877,7 +3872,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3">
       <c r="A40" s="2" t="s">
         <v>48</v>
       </c>
@@ -3888,7 +3883,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3">
       <c r="A41" s="2" t="s">
         <v>48</v>
       </c>
@@ -3899,7 +3894,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3">
       <c r="A42" s="2" t="s">
         <v>52</v>
       </c>
@@ -3910,7 +3905,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3">
       <c r="A43" s="2" t="s">
         <v>52</v>
       </c>
@@ -3921,7 +3916,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3">
       <c r="A44" s="2" t="s">
         <v>52</v>
       </c>
@@ -3932,7 +3927,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3">
       <c r="A45" s="2" t="s">
         <v>52</v>
       </c>
@@ -3943,7 +3938,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3">
       <c r="A46" s="2" t="s">
         <v>97</v>
       </c>
@@ -3954,7 +3949,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3">
       <c r="A47" s="2" t="s">
         <v>97</v>
       </c>
@@ -3965,7 +3960,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3">
       <c r="A48" s="2" t="s">
         <v>97</v>
       </c>
@@ -3976,7 +3971,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3">
       <c r="A49" s="2" t="s">
         <v>97</v>
       </c>
@@ -3987,7 +3982,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3">
       <c r="A50" s="2" t="s">
         <v>94</v>
       </c>
@@ -3998,7 +3993,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3">
       <c r="A51" s="2" t="s">
         <v>94</v>
       </c>
@@ -4009,7 +4004,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3">
       <c r="A52" s="2" t="s">
         <v>94</v>
       </c>
@@ -4020,7 +4015,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3">
       <c r="A53" s="2" t="s">
         <v>94</v>
       </c>
@@ -4031,7 +4026,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3">
       <c r="A54" s="2" t="s">
         <v>56</v>
       </c>
@@ -4042,7 +4037,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3">
       <c r="A55" s="2" t="s">
         <v>56</v>
       </c>
@@ -4053,7 +4048,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3">
       <c r="A56" s="2" t="s">
         <v>70</v>
       </c>
@@ -4064,7 +4059,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3">
       <c r="A57" s="2" t="s">
         <v>70</v>
       </c>
@@ -4075,7 +4070,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3">
       <c r="A58" s="2" t="s">
         <v>70</v>
       </c>
@@ -4086,7 +4081,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3">
       <c r="A59" s="2" t="s">
         <v>74</v>
       </c>
@@ -4097,7 +4092,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3">
       <c r="A60" s="2" t="s">
         <v>74</v>
       </c>
@@ -4108,7 +4103,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3">
       <c r="A61" s="2" t="s">
         <v>74</v>
       </c>
@@ -4119,7 +4114,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3">
       <c r="A62" s="2" t="s">
         <v>74</v>
       </c>
@@ -4130,7 +4125,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3">
       <c r="A63" s="2" t="s">
         <v>74</v>
       </c>
@@ -4141,7 +4136,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3">
       <c r="A64" s="2" t="s">
         <v>74</v>
       </c>
@@ -4152,7 +4147,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3">
       <c r="A65" s="2" t="s">
         <v>74</v>
       </c>
@@ -4163,7 +4158,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3">
       <c r="A66" s="2" t="s">
         <v>71</v>
       </c>
@@ -4174,7 +4169,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:3">
       <c r="A67" s="2" t="s">
         <v>99</v>
       </c>
@@ -4185,7 +4180,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:3">
       <c r="A68" s="2" t="s">
         <v>104</v>
       </c>
@@ -4196,7 +4191,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:3">
       <c r="A69" s="2" t="s">
         <v>104</v>
       </c>
@@ -4207,7 +4202,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:3">
       <c r="A70" s="2" t="s">
         <v>104</v>
       </c>
@@ -4218,7 +4213,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:3">
       <c r="A71" s="2" t="s">
         <v>104</v>
       </c>
@@ -4229,7 +4224,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:3">
       <c r="A72" s="2" t="s">
         <v>104</v>
       </c>
@@ -4240,7 +4235,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:3">
       <c r="A73" s="2" t="s">
         <v>104</v>
       </c>
@@ -4251,7 +4246,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:3">
       <c r="A74" s="2" t="s">
         <v>104</v>
       </c>
@@ -4262,7 +4257,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:3">
       <c r="A75" s="2" t="s">
         <v>104</v>
       </c>
@@ -4273,7 +4268,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:3">
       <c r="A76" s="2" t="s">
         <v>104</v>
       </c>
@@ -4284,7 +4279,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:3">
       <c r="A77" s="2" t="s">
         <v>104</v>
       </c>
@@ -4295,7 +4290,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:3">
       <c r="A78" s="2" t="s">
         <v>114</v>
       </c>
@@ -4306,7 +4301,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:3">
       <c r="A79" s="2" t="s">
         <v>131</v>
       </c>
@@ -4317,7 +4312,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:3">
       <c r="A80" s="2" t="s">
         <v>131</v>
       </c>
@@ -4328,7 +4323,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:3">
       <c r="A81" s="2" t="s">
         <v>131</v>
       </c>
@@ -4339,7 +4334,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:3">
       <c r="A82" s="2" t="s">
         <v>123</v>
       </c>
@@ -4350,7 +4345,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:3">
       <c r="A83" s="2" t="s">
         <v>123</v>
       </c>
@@ -4361,7 +4356,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:3">
       <c r="A84" s="2" t="s">
         <v>144</v>
       </c>
@@ -4372,7 +4367,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:3">
       <c r="A85" s="2" t="s">
         <v>144</v>
       </c>
@@ -4402,13 +4397,13 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="16.33203125" style="2" customWidth="1"/>
-    <col min="2" max="16384" width="10.77734375" style="2"/>
+    <col min="2" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
         <v>191</v>
       </c>
@@ -4419,7 +4414,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="31.45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="30">
       <c r="A2" s="6" t="s">
         <v>136</v>
       </c>
@@ -4427,7 +4422,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
         <v>194</v>
       </c>
@@ -4435,7 +4430,7 @@
         <v>20140512</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="31.45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="30">
       <c r="A4" s="2" t="s">
         <v>195</v>
       </c>
@@ -4443,7 +4438,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="31.45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="30">
       <c r="A5" s="2" t="s">
         <v>197</v>
       </c>
@@ -4470,12 +4465,12 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="52" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2">
       <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
@@ -4483,7 +4478,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2">
       <c r="A2" s="25" t="s">
         <v>13</v>
       </c>
@@ -4491,7 +4486,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2">
       <c r="A3" s="25" t="s">
         <v>13</v>
       </c>
@@ -4499,7 +4494,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2">
       <c r="A4" s="25" t="s">
         <v>185</v>
       </c>
@@ -4507,7 +4502,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2">
       <c r="A5" s="26" t="s">
         <v>12</v>
       </c>
@@ -4515,7 +4510,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2">
       <c r="A6" s="27" t="s">
         <v>13</v>
       </c>
@@ -4523,7 +4518,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2">
       <c r="A7" s="27" t="s">
         <v>14</v>
       </c>
@@ -4531,7 +4526,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2">
       <c r="A8" s="27" t="s">
         <v>14</v>
       </c>
@@ -4539,7 +4534,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2">
       <c r="A9" s="27" t="s">
         <v>185</v>
       </c>
@@ -4547,7 +4542,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2">
       <c r="A10" s="27" t="s">
         <v>218</v>
       </c>
@@ -4555,7 +4550,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2">
       <c r="A11" s="27" t="s">
         <v>185</v>
       </c>
@@ -4563,7 +4558,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2">
       <c r="A12" s="27" t="s">
         <v>218</v>
       </c>
@@ -4571,7 +4566,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2">
       <c r="A13" s="27" t="s">
         <v>12</v>
       </c>
@@ -4579,7 +4574,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2">
       <c r="A14" s="27" t="s">
         <v>185</v>
       </c>
@@ -4587,7 +4582,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2">
       <c r="A15" s="27" t="s">
         <v>12</v>
       </c>
@@ -4595,7 +4590,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2">
       <c r="A16" s="27" t="s">
         <v>185</v>
       </c>
@@ -4603,7 +4598,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2">
       <c r="A17" s="27" t="s">
         <v>185</v>
       </c>
@@ -4611,7 +4606,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="31.45" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" ht="30">
       <c r="A18" s="27" t="s">
         <v>187</v>
       </c>
@@ -4619,7 +4614,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2">
       <c r="A19" s="27" t="s">
         <v>12</v>
       </c>
@@ -4627,7 +4622,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2">
       <c r="A20" s="27" t="s">
         <v>185</v>
       </c>
@@ -4635,7 +4630,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2">
       <c r="A21" s="27" t="s">
         <v>185</v>
       </c>
@@ -4643,7 +4638,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2">
       <c r="A22" s="27" t="s">
         <v>13</v>
       </c>
@@ -4651,7 +4646,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2">
       <c r="A23" s="27" t="s">
         <v>185</v>
       </c>
@@ -4659,7 +4654,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="31.45" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" ht="30">
       <c r="A24" s="27" t="s">
         <v>187</v>
       </c>
@@ -4667,7 +4662,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2">
       <c r="A25" s="27" t="s">
         <v>12</v>
       </c>
@@ -4675,7 +4670,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2">
       <c r="A26" s="27" t="s">
         <v>185</v>
       </c>
@@ -4683,7 +4678,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2">
       <c r="A27" s="27" t="s">
         <v>185</v>
       </c>
@@ -4691,7 +4686,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2">
       <c r="A28" s="27" t="s">
         <v>185</v>
       </c>
@@ -4699,7 +4694,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2">
       <c r="A29" s="27" t="s">
         <v>13</v>
       </c>
@@ -4707,7 +4702,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2">
       <c r="A30" s="27" t="s">
         <v>185</v>
       </c>
@@ -4715,7 +4710,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2">
       <c r="A31" s="27" t="s">
         <v>185</v>
       </c>
@@ -4723,7 +4718,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2">
       <c r="A32" s="27" t="s">
         <v>185</v>
       </c>
@@ -4731,7 +4726,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2">
       <c r="A33" s="27" t="s">
         <v>185</v>
       </c>
@@ -4739,7 +4734,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2">
       <c r="A34" s="27" t="s">
         <v>186</v>
       </c>
@@ -4747,7 +4742,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2">
       <c r="A35" s="27" t="s">
         <v>186</v>
       </c>
@@ -4755,7 +4750,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2">
       <c r="A36" s="27" t="s">
         <v>185</v>
       </c>
@@ -4763,7 +4758,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2">
       <c r="A37" s="27" t="s">
         <v>185</v>
       </c>
@@ -4771,7 +4766,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2">
       <c r="A38" s="27" t="s">
         <v>185</v>
       </c>
@@ -4779,7 +4774,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2">
       <c r="A39" s="27" t="s">
         <v>185</v>
       </c>
@@ -4787,7 +4782,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="31.45" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" ht="30">
       <c r="A40" s="27" t="s">
         <v>187</v>
       </c>
@@ -4795,7 +4790,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2">
       <c r="A41" s="27" t="s">
         <v>12</v>
       </c>
@@ -4803,7 +4798,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2">
       <c r="A42" s="27" t="s">
         <v>185</v>
       </c>
@@ -4811,7 +4806,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="31.45" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" ht="30">
       <c r="A43" s="27" t="s">
         <v>187</v>
       </c>
@@ -4819,7 +4814,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2">
       <c r="A44" s="27" t="s">
         <v>12</v>
       </c>
@@ -4827,7 +4822,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2">
       <c r="A45" s="27" t="s">
         <v>12</v>
       </c>
@@ -4835,7 +4830,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2">
       <c r="A46" s="28" t="s">
         <v>185</v>
       </c>
@@ -4843,7 +4838,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2">
       <c r="A47" s="28" t="s">
         <v>185</v>
       </c>
@@ -4851,7 +4846,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2">
       <c r="A48" s="29" t="s">
         <v>185</v>
       </c>
@@ -4859,7 +4854,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2">
       <c r="A49" s="29" t="s">
         <v>185</v>
       </c>
@@ -4867,7 +4862,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2">
       <c r="A50" s="29" t="s">
         <v>13</v>
       </c>
@@ -4875,7 +4870,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:2">
       <c r="A51" s="29" t="s">
         <v>185</v>
       </c>
@@ -4883,7 +4878,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:2">
       <c r="A52" s="29" t="s">
         <v>12</v>
       </c>
@@ -4891,7 +4886,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:2">
       <c r="A53" s="29" t="s">
         <v>186</v>
       </c>
@@ -4899,7 +4894,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:2">
       <c r="A54" s="29" t="s">
         <v>185</v>
       </c>
@@ -4907,7 +4902,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:2">
       <c r="A55" s="29" t="s">
         <v>12</v>
       </c>
@@ -4915,7 +4910,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="31.45" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:2" ht="30">
       <c r="A56" s="29" t="s">
         <v>187</v>
       </c>
@@ -4923,7 +4918,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:2">
       <c r="A57" s="29" t="s">
         <v>12</v>
       </c>
@@ -4931,7 +4926,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:2">
       <c r="A58" s="29" t="s">
         <v>185</v>
       </c>
@@ -4939,7 +4934,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:2">
       <c r="A59" s="29" t="s">
         <v>13</v>
       </c>
@@ -4947,7 +4942,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:2">
       <c r="A60" s="29" t="s">
         <v>13</v>
       </c>
@@ -4955,7 +4950,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:2">
       <c r="A61" s="29" t="s">
         <v>13</v>
       </c>
@@ -4963,7 +4958,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:2">
       <c r="A62" s="29" t="s">
         <v>185</v>
       </c>
@@ -4971,7 +4966,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:2">
       <c r="A63" s="29" t="s">
         <v>185</v>
       </c>
@@ -4979,7 +4974,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="64" spans="1:2" ht="31.45" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:2" ht="30">
       <c r="A64" s="29" t="s">
         <v>188</v>
       </c>
@@ -4987,7 +4982,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:2">
       <c r="A65" s="29" t="s">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
Add skip logic so that screening form has reasonable flow
</commit_message>
<xml_diff>
--- a/app/config/tables/femaleClients/forms/screenClient/screenClient.xlsx
+++ b/app/config/tables/femaleClients/forms/screenClient/screenClient.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="287">
   <si>
     <t>type</t>
   </si>
@@ -312,9 +312,6 @@
   </si>
   <si>
     <t>relationship_status_options</t>
-  </si>
-  <si>
-    <t xml:space="preserve">How many times have you been pregnant? </t>
   </si>
   <si>
     <t>What was the result of your last HIV test?</t>
@@ -799,9 +796,6 @@
     <t>condition</t>
   </si>
   <si>
-    <t>else</t>
-  </si>
-  <si>
     <t>end if // screening</t>
   </si>
   <si>
@@ -829,21 +823,9 @@
     <t>selected(data('agree_screening'),'a0')</t>
   </si>
   <si>
-    <t>selected(data('curr_relationship'),'a0')</t>
-  </si>
-  <si>
-    <t>data('partner_age') &lt; 18</t>
-  </si>
-  <si>
-    <t>selected(data('clinic_proximity'),'a0')</t>
-  </si>
-  <si>
     <t>goto refuse</t>
   </si>
   <si>
-    <t>selected(data('study_participation'),'a0')</t>
-  </si>
-  <si>
     <t>goto ending</t>
   </si>
   <si>
@@ -853,10 +835,61 @@
     <t>if // ref_reason</t>
   </si>
   <si>
-    <t>selected(data('refusal_reasons','a9')</t>
-  </si>
-  <si>
     <t>end if // ref_reason</t>
+  </si>
+  <si>
+    <t>selected(data('agree_screening'),'a1')</t>
+  </si>
+  <si>
+    <t>selected(data('agree_screening'),'a1') &amp;&amp; (data('age') &gt;= 14)</t>
+  </si>
+  <si>
+    <t>selected(data('agree_screening'),'a1') &amp;&amp; (data('age') &gt;= 14) &amp;&amp; selected(data('pregnant'),'a1') &amp;&amp; selected(data('curr_relationship'),'a1')</t>
+  </si>
+  <si>
+    <t>selected(data('agree_screening'),'a1') &amp;&amp; (data('age') &gt;= 14) &amp;&amp; selected(data('pregnant'),'a1')</t>
+  </si>
+  <si>
+    <t>selected(data('refusal_reasons'),'a9')</t>
+  </si>
+  <si>
+    <t>else // screening</t>
+  </si>
+  <si>
+    <t>selected(data('client_consent'),'a0')</t>
+  </si>
+  <si>
+    <t>selected(data('agree_screening'),'a1') &amp;&amp; (data('age') &gt;= 14) &amp;&amp; selected(data('pregnant'),'a1') &amp;&amp; (data('times_pregnant') &gt; 0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">How many times have you been pregnant before this time? </t>
+  </si>
+  <si>
+    <t>selected(data('agree_screening'),'a0') || (data('age') &lt; 14) || selected(data('pregnant'),'a0') || selected(data('curr_relationship'),'a0') || (data('partner_age') &lt; 18) || selected(data('clinic_proximity'),'a0')</t>
+  </si>
+  <si>
+    <t>selected(data('agree_screening'),'a1') &amp;&amp; (data('age') &gt;= 14) &amp;&amp; selected(data('pregnant'),'a1') &amp;&amp; selected(data('curr_relationship'),'a1') &amp;&amp; (data('partner_age') &gt;= 18) &amp;&amp; selected(data('clinic_proximity'),'a1') &amp;&amp; selected(data('client_consent'),'a1')</t>
+  </si>
+  <si>
+    <t>if // partner</t>
+  </si>
+  <si>
+    <t>end if // partner</t>
+  </si>
+  <si>
+    <t>end if // prior_preg</t>
+  </si>
+  <si>
+    <t>if // prior_preg</t>
+  </si>
+  <si>
+    <t>if // hiv_tested</t>
+  </si>
+  <si>
+    <t>end if // hiv_tested</t>
+  </si>
+  <si>
+    <t>selected(data('hiv_tested'),'a1')</t>
   </si>
 </sst>
 </file>
@@ -2471,13 +2504,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S114"/>
+  <dimension ref="A1:S118"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="G38" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="1" topLeftCell="G29" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B49" sqref="B49"/>
+      <selection pane="bottomRight" activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
@@ -2485,13 +2518,13 @@
     <col min="1" max="1" width="15.44140625" style="3" customWidth="1"/>
     <col min="2" max="2" width="21.44140625" style="3" customWidth="1"/>
     <col min="3" max="3" width="41.21875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" style="8" customWidth="1"/>
-    <col min="5" max="5" width="24.44140625" style="18" customWidth="1"/>
+    <col min="4" max="4" width="21.5546875" style="8" customWidth="1"/>
+    <col min="5" max="5" width="28.33203125" style="18" customWidth="1"/>
     <col min="6" max="6" width="25.109375" style="21" customWidth="1"/>
     <col min="7" max="7" width="63" style="3" customWidth="1"/>
     <col min="8" max="8" width="22.77734375" style="3" customWidth="1"/>
     <col min="9" max="10" width="10.77734375" style="3"/>
-    <col min="11" max="11" width="10.77734375" style="23"/>
+    <col min="11" max="11" width="43.109375" style="23" customWidth="1"/>
     <col min="12" max="12" width="10.77734375" style="3"/>
     <col min="13" max="13" width="15" style="3" customWidth="1"/>
     <col min="14" max="14" width="10.77734375" style="3"/>
@@ -2501,28 +2534,28 @@
   <sheetData>
     <row r="1" spans="1:19" s="5" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D1" s="7" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="17" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F1" s="34" t="s">
         <v>1</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I1" s="5" t="s">
         <v>2</v>
@@ -2564,7 +2597,7 @@
       </c>
       <c r="E2" s="18"/>
       <c r="F2" s="20" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G2" s="11" t="s">
         <v>85</v>
@@ -2579,7 +2612,7 @@
       </c>
       <c r="E3" s="18"/>
       <c r="F3" s="21" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G3" s="13" t="s">
         <v>54</v>
@@ -2605,36 +2638,36 @@
       </c>
       <c r="E5" s="18"/>
       <c r="F5" s="21" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G5" s="13" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="K5" s="31"/>
     </row>
     <row r="6" spans="1:19" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D6" s="8" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E6" s="18" t="s">
         <v>17</v>
       </c>
       <c r="F6" s="21" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G6" s="13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K6" s="31" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:19" s="13" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B7" s="13" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D7" s="8"/>
       <c r="E7" s="18"/>
@@ -2647,10 +2680,10 @@
       </c>
       <c r="E8" s="18"/>
       <c r="F8" s="21" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G8" s="13" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H8" s="13" t="s">
         <v>84</v>
@@ -2659,7 +2692,7 @@
     </row>
     <row r="9" spans="1:19" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B9" s="13" t="s">
-        <v>256</v>
+        <v>274</v>
       </c>
       <c r="D9" s="8"/>
       <c r="E9" s="18"/>
@@ -2672,24 +2705,24 @@
       </c>
       <c r="E10" s="18"/>
       <c r="F10" s="21" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G10" s="13" t="s">
         <v>20</v>
       </c>
       <c r="H10" s="13" t="s">
-        <v>151</v>
-      </c>
-      <c r="K10" s="31" t="b">
-        <v>1</v>
+        <v>150</v>
+      </c>
+      <c r="K10" s="13" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="11" spans="1:19" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B11" s="13" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D11" s="8"/>
       <c r="E11" s="18"/>
@@ -2698,30 +2731,30 @@
     </row>
     <row r="12" spans="1:19" s="13" customFormat="1" ht="47.15" x14ac:dyDescent="0.3">
       <c r="D12" s="8" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E12" s="18" t="s">
         <v>17</v>
       </c>
       <c r="F12" s="21" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G12" s="13" t="s">
         <v>21</v>
       </c>
       <c r="H12" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="K12" s="31" t="b">
-        <v>1</v>
+        <v>112</v>
+      </c>
+      <c r="K12" s="13" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="13" spans="1:19" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B13" s="13" t="s">
+        <v>260</v>
+      </c>
+      <c r="C13" s="13" t="s">
         <v>262</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>264</v>
       </c>
       <c r="D13" s="8"/>
       <c r="E13" s="18"/>
@@ -2734,17 +2767,17 @@
       </c>
       <c r="E14" s="18"/>
       <c r="F14" s="21" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G14" s="13" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K14" s="31"/>
       <c r="N14" s="14"/>
     </row>
     <row r="15" spans="1:19" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B15" s="13" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D15" s="8"/>
       <c r="E15" s="18"/>
@@ -2754,16 +2787,16 @@
     </row>
     <row r="16" spans="1:19" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D16" s="8" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E16" s="18" t="s">
         <v>22</v>
       </c>
       <c r="F16" s="21" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G16" s="13" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K16" s="31"/>
     </row>
@@ -2773,31 +2806,31 @@
       </c>
       <c r="E17" s="18"/>
       <c r="F17" s="21" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G17" s="13" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K17" s="31"/>
     </row>
     <row r="18" spans="2:11" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D18" s="8" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E18" s="18" t="s">
         <v>74</v>
       </c>
       <c r="F18" s="21" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G18" s="15" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K18" s="32"/>
     </row>
     <row r="19" spans="2:11" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D19" s="8" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E19" s="18" t="s">
         <v>29</v>
@@ -2816,22 +2849,22 @@
       </c>
       <c r="E20" s="18"/>
       <c r="F20" s="21" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G20" s="13" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K20" s="31"/>
     </row>
     <row r="21" spans="2:11" s="13" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
       <c r="D21" s="8" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E21" s="18" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F21" s="21" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G21" s="13" t="s">
         <v>40</v>
@@ -2844,16 +2877,16 @@
       </c>
       <c r="E22" s="18"/>
       <c r="F22" s="21" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G22" s="13" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K22" s="31"/>
     </row>
     <row r="23" spans="2:11" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B23" s="13" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D23" s="8"/>
       <c r="E23" s="18"/>
@@ -2862,35 +2895,34 @@
     </row>
     <row r="24" spans="2:11" s="13" customFormat="1" ht="62.85" x14ac:dyDescent="0.3">
       <c r="D24" s="8" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E24" s="18" t="s">
         <v>17</v>
       </c>
       <c r="F24" s="21" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G24" s="13" t="s">
         <v>55</v>
       </c>
       <c r="H24" s="13" t="s">
-        <v>117</v>
-      </c>
-      <c r="K24" s="32" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="2:11" s="13" customFormat="1" x14ac:dyDescent="0.3">
+        <v>116</v>
+      </c>
+      <c r="K24" s="13" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11" s="13" customFormat="1" ht="70.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="13" t="s">
-        <v>262</v>
+        <v>280</v>
       </c>
       <c r="C25" s="13" t="s">
-        <v>266</v>
+        <v>271</v>
       </c>
       <c r="D25" s="8"/>
       <c r="E25" s="18"/>
       <c r="F25" s="21"/>
-      <c r="K25" s="32"/>
     </row>
     <row r="26" spans="2:11" s="13" customFormat="1" ht="94.25" x14ac:dyDescent="0.3">
       <c r="D26" s="8" t="s">
@@ -2898,31 +2930,27 @@
       </c>
       <c r="E26" s="18"/>
       <c r="F26" s="21" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G26" s="13" t="s">
         <v>73</v>
       </c>
       <c r="H26" s="13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J26" s="16"/>
-      <c r="K26" s="31" t="b">
-        <v>1</v>
+      <c r="K26" s="13" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="27" spans="2:11" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B27" s="13" t="s">
-        <v>262</v>
-      </c>
-      <c r="C27" s="13" t="s">
-        <v>267</v>
+        <v>281</v>
       </c>
       <c r="D27" s="8"/>
       <c r="E27" s="18"/>
       <c r="F27" s="21"/>
       <c r="J27" s="16"/>
-      <c r="K27" s="31"/>
     </row>
     <row r="28" spans="2:11" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D28" s="8" t="s">
@@ -2930,313 +2958,345 @@
       </c>
       <c r="E28" s="18"/>
       <c r="F28" s="21" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G28" s="13" t="s">
-        <v>95</v>
+        <v>277</v>
       </c>
       <c r="K28" s="32"/>
     </row>
-    <row r="29" spans="2:11" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="D29" s="8" t="s">
-        <v>13</v>
-      </c>
+    <row r="29" spans="2:11" s="13" customFormat="1" ht="62.85" x14ac:dyDescent="0.3">
+      <c r="B29" s="13" t="s">
+        <v>283</v>
+      </c>
+      <c r="C29" s="32" t="s">
+        <v>276</v>
+      </c>
+      <c r="D29" s="8"/>
       <c r="E29" s="18"/>
-      <c r="F29" s="21" t="s">
-        <v>171</v>
-      </c>
-      <c r="G29" s="13" t="s">
-        <v>81</v>
-      </c>
+      <c r="F29" s="21"/>
       <c r="K29" s="32"/>
     </row>
     <row r="30" spans="2:11" s="13" customFormat="1" ht="62.85" x14ac:dyDescent="0.3">
       <c r="D30" s="8" t="s">
-        <v>185</v>
-      </c>
-      <c r="E30" s="18" t="s">
-        <v>17</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="E30" s="18"/>
       <c r="F30" s="21" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="G30" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="H30" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="K30" s="32" t="b">
-        <v>1</v>
+        <v>81</v>
+      </c>
+      <c r="K30" s="32" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="31" spans="2:11" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B31" s="13" t="s">
-        <v>262</v>
-      </c>
-      <c r="C31" s="13" t="s">
-        <v>268</v>
+        <v>282</v>
       </c>
       <c r="D31" s="8"/>
       <c r="E31" s="18"/>
       <c r="F31" s="21"/>
       <c r="K31" s="32"/>
     </row>
-    <row r="32" spans="2:11" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:11" s="13" customFormat="1" ht="62.85" x14ac:dyDescent="0.3">
       <c r="D32" s="8" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E32" s="18" t="s">
-        <v>121</v>
+        <v>17</v>
       </c>
       <c r="F32" s="21" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="G32" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="K32" s="32"/>
+        <v>47</v>
+      </c>
+      <c r="H32" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="K32" s="13" t="s">
+        <v>272</v>
+      </c>
     </row>
     <row r="33" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D33" s="8" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E33" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="F33" s="21" t="s">
+        <v>172</v>
+      </c>
+      <c r="G33" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="K33" s="32"/>
+    </row>
+    <row r="34" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="C34" s="13" t="s">
+        <v>286</v>
+      </c>
+      <c r="D34" s="8"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="21"/>
+      <c r="K34" s="32"/>
+    </row>
+    <row r="35" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D35" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="E35" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="F33" s="21" t="s">
-        <v>174</v>
-      </c>
-      <c r="G33" s="13" t="s">
-        <v>96</v>
-      </c>
-      <c r="K33" s="32"/>
-    </row>
-    <row r="34" spans="1:11" s="13" customFormat="1" ht="47.15" x14ac:dyDescent="0.3">
-      <c r="D34" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E34" s="19"/>
-      <c r="F34" s="21" t="s">
-        <v>176</v>
-      </c>
-      <c r="G34" s="13" t="s">
-        <v>134</v>
-      </c>
-      <c r="H34" s="13" t="s">
-        <v>102</v>
-      </c>
-      <c r="K34" s="31"/>
-    </row>
-    <row r="35" spans="1:11" s="13" customFormat="1" ht="47.15" x14ac:dyDescent="0.3">
-      <c r="D35" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="E35" s="19" t="s">
-        <v>123</v>
-      </c>
       <c r="F35" s="21" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="G35" s="13" t="s">
-        <v>140</v>
-      </c>
-      <c r="H35" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="K35" s="31"/>
+        <v>95</v>
+      </c>
+      <c r="K35" s="32"/>
     </row>
     <row r="36" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B36" s="13" t="s">
-        <v>269</v>
-      </c>
-      <c r="C36" s="13" t="s">
-        <v>270</v>
-      </c>
-      <c r="D36" s="9"/>
-      <c r="E36" s="19"/>
+        <v>285</v>
+      </c>
+      <c r="D36" s="8"/>
+      <c r="E36" s="18"/>
       <c r="F36" s="21"/>
-      <c r="K36" s="31"/>
-    </row>
-    <row r="37" spans="1:11" s="13" customFormat="1" ht="47.15" x14ac:dyDescent="0.3">
-      <c r="D37" s="8" t="s">
-        <v>13</v>
-      </c>
+      <c r="K36" s="32"/>
+    </row>
+    <row r="37" spans="1:11" s="13" customFormat="1" ht="94.25" x14ac:dyDescent="0.3">
+      <c r="B37" s="13" t="s">
+        <v>260</v>
+      </c>
+      <c r="C37" s="13" t="s">
+        <v>278</v>
+      </c>
+      <c r="D37" s="8"/>
       <c r="E37" s="18"/>
-      <c r="F37" s="21" t="s">
-        <v>178</v>
-      </c>
-      <c r="G37" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="H37" s="13" t="s">
-        <v>142</v>
-      </c>
-      <c r="K37" s="32" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="D38" s="8" t="s">
-        <v>185</v>
-      </c>
-      <c r="E38" s="18" t="s">
-        <v>144</v>
-      </c>
+      <c r="F37" s="21"/>
+      <c r="K37" s="32"/>
+    </row>
+    <row r="38" spans="1:11" s="13" customFormat="1" ht="47.15" x14ac:dyDescent="0.3">
+      <c r="D38" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E38" s="19"/>
       <c r="F38" s="21" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="G38" s="13" t="s">
-        <v>143</v>
-      </c>
-      <c r="K38" s="31" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="3" t="s">
-        <v>257</v>
-      </c>
-      <c r="D39" s="8"/>
-      <c r="E39" s="18"/>
-      <c r="F39" s="21"/>
+        <v>133</v>
+      </c>
+      <c r="H38" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="K38" s="31"/>
+    </row>
+    <row r="39" spans="1:11" s="13" customFormat="1" ht="47.15" x14ac:dyDescent="0.3">
+      <c r="D39" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="E39" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="F39" s="21" t="s">
+        <v>176</v>
+      </c>
+      <c r="G39" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="H39" s="13" t="s">
+        <v>53</v>
+      </c>
       <c r="K39" s="31"/>
     </row>
     <row r="40" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B40" s="13" t="s">
-        <v>271</v>
-      </c>
-      <c r="D40" s="8"/>
-      <c r="E40" s="18"/>
+        <v>264</v>
+      </c>
+      <c r="C40" s="13" t="s">
+        <v>275</v>
+      </c>
+      <c r="D40" s="9"/>
+      <c r="E40" s="19"/>
       <c r="F40" s="21"/>
-      <c r="K40" s="32"/>
-    </row>
-    <row r="41" spans="1:11" s="13" customFormat="1" ht="62.85" x14ac:dyDescent="0.3">
-      <c r="A41" s="13" t="s">
-        <v>260</v>
-      </c>
-      <c r="D41" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E41" s="19"/>
+      <c r="K40" s="31"/>
+    </row>
+    <row r="41" spans="1:11" s="13" customFormat="1" ht="110" x14ac:dyDescent="0.3">
+      <c r="D41" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E41" s="18"/>
       <c r="F41" s="21" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="G41" s="13" t="s">
-        <v>139</v>
-      </c>
-      <c r="K41" s="31"/>
-    </row>
-    <row r="42" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="13" t="s">
-        <v>271</v>
-      </c>
-      <c r="D42" s="9"/>
-      <c r="E42" s="19"/>
-      <c r="F42" s="21"/>
-      <c r="K42" s="31"/>
-    </row>
-    <row r="43" spans="1:11" s="13" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
-      <c r="A43" s="13" t="s">
-        <v>261</v>
-      </c>
-      <c r="D43" s="8" t="s">
-        <v>188</v>
-      </c>
-      <c r="E43" s="18" t="s">
-        <v>104</v>
-      </c>
-      <c r="F43" s="21" t="s">
-        <v>180</v>
-      </c>
-      <c r="G43" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="K43" s="32"/>
+        <v>140</v>
+      </c>
+      <c r="H41" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="K41" s="13" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" s="13" customFormat="1" ht="110" x14ac:dyDescent="0.3">
+      <c r="D42" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="E42" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="F42" s="21" t="s">
+        <v>178</v>
+      </c>
+      <c r="G42" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="K42" s="13" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B43" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="D43" s="8"/>
+      <c r="E43" s="18"/>
+      <c r="F43" s="21"/>
+      <c r="K43" s="31"/>
     </row>
     <row r="44" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B44" s="13" t="s">
-        <v>273</v>
-      </c>
-      <c r="C44" s="13" t="s">
-        <v>274</v>
+        <v>265</v>
       </c>
       <c r="D44" s="8"/>
       <c r="E44" s="18"/>
       <c r="F44" s="21"/>
       <c r="K44" s="32"/>
     </row>
-    <row r="45" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="D45" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="E45" s="18"/>
+    <row r="45" spans="1:11" s="13" customFormat="1" ht="62.85" x14ac:dyDescent="0.3">
+      <c r="A45" s="13" t="s">
+        <v>258</v>
+      </c>
+      <c r="D45" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E45" s="19"/>
       <c r="F45" s="21" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="G45" s="13" t="s">
-        <v>125</v>
-      </c>
-      <c r="K45" s="32"/>
+        <v>138</v>
+      </c>
+      <c r="K45" s="31"/>
     </row>
     <row r="46" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B46" s="13" t="s">
-        <v>275</v>
-      </c>
-      <c r="D46" s="8"/>
-      <c r="E46" s="18"/>
+        <v>265</v>
+      </c>
+      <c r="D46" s="9"/>
+      <c r="E46" s="19"/>
       <c r="F46" s="21"/>
-      <c r="K46" s="32"/>
-    </row>
-    <row r="47" spans="1:11" s="13" customFormat="1" ht="62.85" x14ac:dyDescent="0.3">
-      <c r="D47" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E47" s="19"/>
+      <c r="K46" s="31"/>
+    </row>
+    <row r="47" spans="1:11" s="13" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
+      <c r="A47" s="13" t="s">
+        <v>259</v>
+      </c>
+      <c r="D47" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="E47" s="18" t="s">
+        <v>103</v>
+      </c>
       <c r="F47" s="21" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="G47" s="13" t="s">
-        <v>150</v>
-      </c>
-      <c r="K47" s="31"/>
+        <v>102</v>
+      </c>
+      <c r="K47" s="32"/>
     </row>
     <row r="48" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B48" s="13" t="s">
-        <v>271</v>
+        <v>267</v>
+      </c>
+      <c r="C48" s="13" t="s">
+        <v>273</v>
       </c>
       <c r="D48" s="8"/>
       <c r="E48" s="18"/>
       <c r="F48" s="21"/>
-      <c r="K48" s="31"/>
-    </row>
-    <row r="49" spans="1:11" s="13" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
-      <c r="A49" s="13" t="s">
-        <v>272</v>
-      </c>
+      <c r="K48" s="32"/>
+    </row>
+    <row r="49" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D49" s="8" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E49" s="18"/>
       <c r="F49" s="21" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="G49" s="13" t="s">
-        <v>116</v>
-      </c>
-      <c r="K49" s="31"/>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="K50" s="33"/>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="K51" s="33"/>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="K52" s="33"/>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="K53" s="33"/>
+        <v>124</v>
+      </c>
+      <c r="K49" s="32"/>
+    </row>
+    <row r="50" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B50" s="13" t="s">
+        <v>268</v>
+      </c>
+      <c r="D50" s="8"/>
+      <c r="E50" s="18"/>
+      <c r="F50" s="21"/>
+      <c r="K50" s="32"/>
+    </row>
+    <row r="51" spans="1:11" s="13" customFormat="1" ht="62.85" x14ac:dyDescent="0.3">
+      <c r="D51" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E51" s="19"/>
+      <c r="F51" s="21" t="s">
+        <v>181</v>
+      </c>
+      <c r="G51" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="K51" s="31"/>
+    </row>
+    <row r="52" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B52" s="13" t="s">
+        <v>265</v>
+      </c>
+      <c r="D52" s="8"/>
+      <c r="E52" s="18"/>
+      <c r="F52" s="21"/>
+      <c r="K52" s="31"/>
+    </row>
+    <row r="53" spans="1:11" s="13" customFormat="1" ht="31.45" x14ac:dyDescent="0.3">
+      <c r="A53" s="13" t="s">
+        <v>266</v>
+      </c>
+      <c r="D53" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E53" s="18"/>
+      <c r="F53" s="21" t="s">
+        <v>182</v>
+      </c>
+      <c r="G53" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="K53" s="31"/>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K54" s="33"/>
@@ -3420,6 +3480,18 @@
     </row>
     <row r="114" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K114" s="33"/>
+    </row>
+    <row r="115" spans="11:11" x14ac:dyDescent="0.3">
+      <c r="K115" s="33"/>
+    </row>
+    <row r="116" spans="11:11" x14ac:dyDescent="0.3">
+      <c r="K116" s="33"/>
+    </row>
+    <row r="117" spans="11:11" x14ac:dyDescent="0.3">
+      <c r="K117" s="33"/>
+    </row>
+    <row r="118" spans="11:11" x14ac:dyDescent="0.3">
+      <c r="K118" s="33"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3436,8 +3508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C85"/>
   <sheetViews>
-    <sheetView topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.44140625" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
@@ -3450,13 +3522,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>190</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -3464,7 +3536,7 @@
         <v>17</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>18</v>
@@ -3475,7 +3547,7 @@
         <v>17</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>19</v>
@@ -3483,10 +3555,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>18</v>
@@ -3494,10 +3566,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>19</v>
@@ -3505,10 +3577,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>86</v>
@@ -3516,10 +3588,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>86</v>
@@ -3530,7 +3602,7 @@
         <v>22</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>23</v>
@@ -3541,7 +3613,7 @@
         <v>22</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>24</v>
@@ -3552,7 +3624,7 @@
         <v>22</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>25</v>
@@ -3563,7 +3635,7 @@
         <v>22</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>26</v>
@@ -3574,7 +3646,7 @@
         <v>22</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>27</v>
@@ -3585,7 +3657,7 @@
         <v>22</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>28</v>
@@ -3596,7 +3668,7 @@
         <v>22</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>69</v>
@@ -3607,7 +3679,7 @@
         <v>22</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>86</v>
@@ -3618,7 +3690,7 @@
         <v>29</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>31</v>
@@ -3629,7 +3701,7 @@
         <v>29</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>32</v>
@@ -3640,7 +3712,7 @@
         <v>29</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>33</v>
@@ -3651,7 +3723,7 @@
         <v>29</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>34</v>
@@ -3662,7 +3734,7 @@
         <v>29</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>35</v>
@@ -3673,7 +3745,7 @@
         <v>29</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>36</v>
@@ -3684,7 +3756,7 @@
         <v>29</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>37</v>
@@ -3695,7 +3767,7 @@
         <v>29</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>38</v>
@@ -3706,7 +3778,7 @@
         <v>29</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>30</v>
@@ -3717,7 +3789,7 @@
         <v>29</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>69</v>
@@ -3728,7 +3800,7 @@
         <v>29</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>86</v>
@@ -3736,10 +3808,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>87</v>
@@ -3747,10 +3819,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>88</v>
@@ -3758,10 +3830,10 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>45</v>
@@ -3769,10 +3841,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>42</v>
@@ -3780,10 +3852,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>43</v>
@@ -3791,10 +3863,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>89</v>
@@ -3802,10 +3874,10 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>44</v>
@@ -3813,10 +3885,10 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>46</v>
@@ -3824,10 +3896,10 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>41</v>
@@ -3835,10 +3907,10 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>69</v>
@@ -3846,10 +3918,10 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>86</v>
@@ -3860,7 +3932,7 @@
         <v>48</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>49</v>
@@ -3871,7 +3943,7 @@
         <v>48</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>50</v>
@@ -3882,7 +3954,7 @@
         <v>48</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>69</v>
@@ -3893,7 +3965,7 @@
         <v>48</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>86</v>
@@ -3904,7 +3976,7 @@
         <v>52</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>64</v>
@@ -3915,7 +3987,7 @@
         <v>52</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>65</v>
@@ -3926,7 +3998,7 @@
         <v>52</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>86</v>
@@ -3937,7 +4009,7 @@
         <v>52</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>82</v>
@@ -3945,10 +4017,10 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>18</v>
@@ -3956,10 +4028,10 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>19</v>
@@ -3967,10 +4039,10 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>86</v>
@@ -3978,10 +4050,10 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>82</v>
@@ -3992,7 +4064,7 @@
         <v>94</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>90</v>
@@ -4003,7 +4075,7 @@
         <v>94</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>91</v>
@@ -4014,7 +4086,7 @@
         <v>94</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>92</v>
@@ -4025,7 +4097,7 @@
         <v>94</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>93</v>
@@ -4091,7 +4163,7 @@
         <v>74</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>75</v>
@@ -4102,7 +4174,7 @@
         <v>74</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>76</v>
@@ -4113,7 +4185,7 @@
         <v>74</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>77</v>
@@ -4124,7 +4196,7 @@
         <v>74</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>78</v>
@@ -4135,7 +4207,7 @@
         <v>74</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C63" s="2" t="s">
         <v>79</v>
@@ -4146,7 +4218,7 @@
         <v>74</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>80</v>
@@ -4157,7 +4229,7 @@
         <v>74</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C65" s="2" t="s">
         <v>86</v>
@@ -4168,7 +4240,7 @@
         <v>71</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C66" s="4" t="s">
         <v>72</v>
@@ -4176,109 +4248,109 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="C67" s="2" t="s">
         <v>99</v>
-      </c>
-      <c r="B67" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="C67" s="2" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="C68" s="2" t="s">
         <v>104</v>
-      </c>
-      <c r="B68" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="C68" s="2" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C76" s="2" t="s">
         <v>69</v>
@@ -4286,10 +4358,10 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C77" s="2" t="s">
         <v>86</v>
@@ -4297,43 +4369,43 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="C80" s="2" t="s">
         <v>131</v>
-      </c>
-      <c r="B80" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="C80" s="2" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C81" s="2" t="s">
         <v>86</v>
@@ -4341,46 +4413,46 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="C83" s="2" t="s">
         <v>123</v>
-      </c>
-      <c r="B83" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="C83" s="2" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C84" s="2" t="s">
         <v>144</v>
-      </c>
-      <c r="B84" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="C84" s="2" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -4410,26 +4482,26 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>192</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="31.45" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>136</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B3" s="2">
         <v>20140512</v>
@@ -4437,18 +4509,18 @@
     </row>
     <row r="4" spans="1:3" ht="31.45" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>195</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="31.45" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>197</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>198</v>
       </c>
     </row>
   </sheetData>
@@ -4488,7 +4560,7 @@
         <v>13</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -4496,15 +4568,15 @@
         <v>13</v>
       </c>
       <c r="B3" s="25" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="25" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -4512,7 +4584,7 @@
         <v>12</v>
       </c>
       <c r="B5" s="27" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -4520,7 +4592,7 @@
         <v>13</v>
       </c>
       <c r="B6" s="27" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -4536,39 +4608,39 @@
         <v>14</v>
       </c>
       <c r="B8" s="27" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="27" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B9" s="27" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="27" t="s">
+        <v>217</v>
+      </c>
+      <c r="B10" s="27" t="s">
         <v>218</v>
-      </c>
-      <c r="B10" s="27" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="27" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B11" s="27" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="27" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B12" s="27" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -4576,15 +4648,15 @@
         <v>12</v>
       </c>
       <c r="B13" s="27" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="27" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B14" s="27" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -4592,31 +4664,31 @@
         <v>12</v>
       </c>
       <c r="B15" s="27" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="27" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B16" s="27" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="27" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B17" s="27" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="31.45" x14ac:dyDescent="0.3">
       <c r="A18" s="27" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B18" s="27" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
@@ -4624,23 +4696,23 @@
         <v>12</v>
       </c>
       <c r="B19" s="27" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="27" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B20" s="27" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="27" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B21" s="27" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
@@ -4648,23 +4720,23 @@
         <v>13</v>
       </c>
       <c r="B22" s="27" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="27" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B23" s="27" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="31.45" x14ac:dyDescent="0.3">
       <c r="A24" s="27" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B24" s="27" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
@@ -4672,31 +4744,31 @@
         <v>12</v>
       </c>
       <c r="B25" s="27" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="27" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B26" s="27" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="27" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B27" s="27" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="27" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B28" s="27" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
@@ -4704,95 +4776,95 @@
         <v>13</v>
       </c>
       <c r="B29" s="27" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="27" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B30" s="27" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="27" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B31" s="27" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="27" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B32" s="27" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="27" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B33" s="27" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="27" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B34" s="27" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="27" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B35" s="27" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="27" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B36" s="27" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="27" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B37" s="27" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="27" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B38" s="27" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="27" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B39" s="27" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="31.45" x14ac:dyDescent="0.3">
       <c r="A40" s="27" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B40" s="27" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
@@ -4800,23 +4872,23 @@
         <v>12</v>
       </c>
       <c r="B41" s="27" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="27" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B42" s="27" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="31.45" x14ac:dyDescent="0.3">
       <c r="A43" s="27" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B43" s="27" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
@@ -4824,7 +4896,7 @@
         <v>12</v>
       </c>
       <c r="B44" s="27" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
@@ -4832,39 +4904,39 @@
         <v>12</v>
       </c>
       <c r="B45" s="27" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" s="28" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B46" s="28" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" s="28" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B47" s="28" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" s="29" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B48" s="29" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="29" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B49" s="29" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
@@ -4872,15 +4944,15 @@
         <v>13</v>
       </c>
       <c r="B50" s="29" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" s="29" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B51" s="29" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
@@ -4888,20 +4960,20 @@
         <v>12</v>
       </c>
       <c r="B52" s="29" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" s="29" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B53" s="29" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" s="29" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B54" s="29" t="s">
         <v>29</v>
@@ -4912,15 +4984,15 @@
         <v>12</v>
       </c>
       <c r="B55" s="29" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="31.45" x14ac:dyDescent="0.3">
       <c r="A56" s="29" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B56" s="29" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
@@ -4928,15 +5000,15 @@
         <v>12</v>
       </c>
       <c r="B57" s="29" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" s="29" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B58" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
@@ -4944,7 +5016,7 @@
         <v>13</v>
       </c>
       <c r="B59" s="29" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
@@ -4952,7 +5024,7 @@
         <v>13</v>
       </c>
       <c r="B60" s="29" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
@@ -4960,31 +5032,31 @@
         <v>13</v>
       </c>
       <c r="B61" s="29" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" s="29" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B62" s="29" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" s="29" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B63" s="29" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="31.45" x14ac:dyDescent="0.3">
       <c r="A64" s="29" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B64" s="29" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
@@ -4992,7 +5064,7 @@
         <v>12</v>
       </c>
       <c r="B65" s="29" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
   </sheetData>

</xml_diff>